<commit_message>
support Jetty, support Cango, support Nexus, change BaseAction to DispatchAction.
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="20120307" sheetId="1" r:id="rId1"/>
     <sheet name="20120308" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="20120309" sheetId="3" r:id="rId3"/>
+    <sheet name="20120725" sheetId="4" r:id="rId4"/>
+    <sheet name="20120727" sheetId="5" r:id="rId5"/>
+    <sheet name="20120728" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>devfw change to Maven</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +78,62 @@
   </si>
   <si>
     <t>1h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOA study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:00-16:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hudson study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:30-18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>firebird study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:00-17:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:00-12:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:00-12:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change BaseAction  to DispatchAction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -492,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F12:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -520,13 +579,142 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="F10:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="6:11" x14ac:dyDescent="0.15">
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G13:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="13" spans="7:13" x14ac:dyDescent="0.15">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G13:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="13" spans="7:13" x14ac:dyDescent="0.15">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E11:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="10" max="10" width="25.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="5:13" x14ac:dyDescent="0.15">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add header.jsp and change all relative URL to the same URL in header.jsp
</commit_message>
<xml_diff>
--- a/Documents/DailyPlan.xlsx
+++ b/Documents/DailyPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="20120307" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="20120725" sheetId="4" r:id="rId4"/>
     <sheet name="20120727" sheetId="5" r:id="rId5"/>
     <sheet name="20120728" sheetId="6" r:id="rId6"/>
+    <sheet name="20120730" sheetId="7" r:id="rId7"/>
+    <sheet name="20120731" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>devfw change to Maven</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,6 +136,26 @@
   </si>
   <si>
     <t>change BaseAction  to DispatchAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fix jetty debug issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fix jetty debug issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>change relative URL to the same URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8h</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -689,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E11:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -717,4 +739,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E11:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="34.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="5:9" x14ac:dyDescent="0.15">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="5:9" x14ac:dyDescent="0.15">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F11:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="11" spans="6:10" x14ac:dyDescent="0.15">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>